<commit_message>
Include scenarios 1 and 3
</commit_message>
<xml_diff>
--- a/Projects/Tanzania/data/optimisationBudgets.xlsx
+++ b/Projects/Tanzania/data/optimisationBudgets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/Projects/Tanzania/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A9F71DD9-1892-CD48-BAE8-D5E7331283B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7CB99022-26C6-B440-8F0F-B8E37EE398EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" activeTab="1" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
   </bookViews>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Region</t>
   </si>
@@ -1058,7 +1058,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1101,7 +1101,9 @@
         <f>(20+30+45+45+35+22)/6 * 1000000</f>
         <v>32833333.333333336</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">

</xml_diff>

<commit_message>
Upped num particles, regions
</commit_message>
<xml_diff>
--- a/Projects/Tanzania/data/optimisationBudgets.xlsx
+++ b/Projects/Tanzania/data/optimisationBudgets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/Projects/Tanzania/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7CB99022-26C6-B440-8F0F-B8E37EE398EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9951DFAA-3EF3-FF47-B7FC-FF5213186AEE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" activeTab="1" xr2:uid="{6937E72E-728A-D145-8CDA-D71DF27F887B}"/>
   </bookViews>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Region</t>
   </si>
@@ -1058,7 +1058,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,9 +1134,7 @@
         <f>(20+30+45+45+35+22)/6 * 1000000</f>
         <v>32833333.333333336</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="E4" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">

</xml_diff>